<commit_message>
support autocloseable on Book. reuse styles.
</commit_message>
<xml_diff>
--- a/output/simplesheet.xlsx
+++ b/output/simplesheet.xlsx
@@ -34,18 +34,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -73,10 +68,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -93,7 +87,7 @@
       <c r="A1" t="s" s="1">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" t="s" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>